<commit_message>
subject - availability,frames,save submit Pending
</commit_message>
<xml_diff>
--- a/testdata/Tutor addsubject.xlsx
+++ b/testdata/Tutor addsubject.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoges\PycharmProjects\ilrnu\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8A17DB-27BD-4E51-8209-A09E75E81248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCD10B8-BE59-443A-92DD-A34CA3C79EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Add subject" sheetId="1" r:id="rId1"/>
+    <sheet name="Addsubject" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Login tutor" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -103,40 +103,40 @@
     <t>India@2020</t>
   </si>
   <si>
-    <t>Subject_name</t>
-  </si>
-  <si>
-    <t>Subject_description</t>
-  </si>
-  <si>
-    <t>Subject_highlights</t>
-  </si>
-  <si>
-    <t>Add_tags</t>
-  </si>
-  <si>
-    <t>Starttime_Hour</t>
-  </si>
-  <si>
-    <t>Starttime_ Min</t>
-  </si>
-  <si>
-    <t>Endtime_Hour</t>
-  </si>
-  <si>
-    <t>Endtime_Min</t>
-  </si>
-  <si>
-    <t>Start_AMPM</t>
-  </si>
-  <si>
-    <t>End_AMPM</t>
-  </si>
-  <si>
-    <t>Individual_price</t>
-  </si>
-  <si>
-    <t>Group_price</t>
+    <t>Subjectname</t>
+  </si>
+  <si>
+    <t>Subjectdescription</t>
+  </si>
+  <si>
+    <t>Subjecthighlights</t>
+  </si>
+  <si>
+    <t>Addtags</t>
+  </si>
+  <si>
+    <t>StarttimeHour</t>
+  </si>
+  <si>
+    <t>EndtimeHour</t>
+  </si>
+  <si>
+    <t>EndtimeMin</t>
+  </si>
+  <si>
+    <t>StartAMPM</t>
+  </si>
+  <si>
+    <t>EndAMPM</t>
+  </si>
+  <si>
+    <t>Individualprice</t>
+  </si>
+  <si>
+    <t>Groupprice</t>
+  </si>
+  <si>
+    <t>StarttimeMin</t>
   </si>
 </sst>
 </file>
@@ -216,11 +216,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -229,6 +226,12 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -570,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,135 +601,136 @@
     <col min="21" max="21" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
         <v>10</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>15</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>12</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>15</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>500</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -740,189 +744,189 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2">
-        <v>1</v>
-      </c>
-      <c r="L1" s="2">
-        <v>1</v>
-      </c>
-      <c r="M1" s="2">
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1">
         <v>6</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>0</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>8</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1">
         <v>0</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>1000</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
         <v>10</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>15</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>12</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>15</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>500</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
         <v>6</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>8</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>0</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="1">
         <v>1000</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="1">
         <v>2000</v>
       </c>
     </row>
@@ -946,24 +950,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>